<commit_message>
Added another classification based on functionalities
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="123">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -64,7 +64,7 @@
     <t>pav:version</t>
   </si>
   <si>
-    <t>0.0.1</t>
+    <t>0.0.2</t>
   </si>
   <si>
     <t>pav:createdOn</t>
@@ -233,6 +233,63 @@
   </si>
   <si>
     <t>An L4 Living Digital Twin focuses on modeling the behavior of the physical system as it changes over time by using real-world data to update the model parameters.</t>
+  </si>
+  <si>
+    <t>ditta:0-StandaloneDigitalTwin</t>
+  </si>
+  <si>
+    <t>Standalone Digital Twin</t>
+  </si>
+  <si>
+    <t>A standalone DT is defined as a DT even before the physical asset comes into existence. The value of a standalone DT, in addition to being used for design purposes, is that it can be used for a preliminary cost-benefit analysis of the asset before it is built.</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0009-0003-5155-0870</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/ACCESS.2023.3321320</t>
+  </si>
+  <si>
+    <t>ditta:1-DescriptiveDigitalTwin</t>
+  </si>
+  <si>
+    <t>Descriptive Digital Twin</t>
+  </si>
+  <si>
+    <t>When geometric computer-aided design (CAD) models are in place and a live sensor data stream is established, it can be referred to as the descriptive DT, which can provide insight into the inner workings of the asset at the required granularity. A descriptive DT mirrors the physical asset’s current state and can be easily explored remotely.</t>
+  </si>
+  <si>
+    <t>ditta:2-DiagnosticDigitalTwin</t>
+  </si>
+  <si>
+    <t>Diagnostic Digital Twin</t>
+  </si>
+  <si>
+    <t>At a capability level of 2, data analysis tools are applied to the data for sanity-checks of sensors and data, condition monitoring and fault diagnosis. The DT is referred to as the diagnostic DT.</t>
+  </si>
+  <si>
+    <t>ditta:3-PredictiveDigitalTwin</t>
+  </si>
+  <si>
+    <t>Predictive Digital Twin</t>
+  </si>
+  <si>
+    <t>Predictive DT, as the name suggests, starts exploiting models to project the current and past states into the future. The prediction is continuously updated based on the real-time data stream from the physical asset. With the constant update of the asset state, there is no risk of diverging too far from the physical asset over time.</t>
+  </si>
+  <si>
+    <t>ditta:4-PrescriptiveDigitalTwin</t>
+  </si>
+  <si>
+    <t>Prescriptive Digital Twin</t>
+  </si>
+  <si>
+    <t>Prescriptive DTs [...] can make recommendations based on what-if? / risk assessment and uncertainty quantification. This aspect is highly desirable for decision support systems, providing recommendations to experts who then decide how to act upon them.</t>
+  </si>
+  <si>
+    <t>ditta:5-AutonomousDigitalTwin</t>
+  </si>
+  <si>
+    <t>The DT and the digital asset start bidirectional communication where the physical asset updates its DT in real-time, and in return, the DT controls the asset to push it towards an optimal set point. Decisions can be made on much shorter timescales than with human involvement. This autonomous DT represents the fifth level.</t>
   </si>
   <si>
     <t>Intelligent Digital Twin</t>
@@ -329,7 +386,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -378,6 +435,10 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -393,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -443,6 +504,7 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -666,7 +728,7 @@
     <col customWidth="1" min="2" max="2" width="40.0"/>
     <col customWidth="1" min="3" max="3" width="43.88"/>
     <col customWidth="1" min="5" max="5" width="29.5"/>
-    <col customWidth="1" min="7" max="7" width="28.5"/>
+    <col customWidth="1" min="7" max="7" width="67.75"/>
     <col customWidth="1" min="9" max="9" width="30.5"/>
     <col customWidth="1" min="10" max="10" width="29.63"/>
     <col customWidth="1" min="11" max="11" width="27.25"/>
@@ -862,7 +924,7 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="3"/>
@@ -996,7 +1058,7 @@
     </row>
     <row r="16">
       <c r="A16" s="11" t="str">
-        <f t="shared" ref="A16:A48" si="1">IF(ISBLANK($B16),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B16," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" ref="A16:A35" si="1">IF(ISBLANK($B16),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B16," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>ditta:DigitalTwinConceptualModel</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -1237,9 +1299,13 @@
         <f t="shared" si="4"/>
         <v>ditta:Intelligent-LearningDigitalTwin</v>
       </c>
+      <c r="F30" s="11" t="str">
+        <f>TEXTJOIN(",",1,A41)</f>
+        <v>ditta:5-AutonomousDigitalTwin</v>
+      </c>
       <c r="G30" s="11" t="str">
-        <f>TEXTJOIN(",",1,A31,A35)</f>
-        <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A31)</f>
+        <v>ditta:CognitiveDigitalTwin</v>
       </c>
       <c r="I30" s="14" t="s">
         <v>55</v>
@@ -1359,291 +1425,451 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>ditta:IntelligentDigitalTwin</v>
+      <c r="A36" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="C36" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="E36" s="11" t="str">
         <f>$A$25</f>
         <v>ditta:SystemFunctionality</v>
       </c>
-      <c r="G36" s="11" t="str">
+      <c r="I36" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="11" t="str">
+        <f t="shared" ref="E37:E41" si="8">A36</f>
+        <v>ditta:0-StandaloneDigitalTwin</v>
+      </c>
+      <c r="G37" s="11" t="str">
+        <f t="shared" ref="G37:G40" si="9">TEXTJOIN(",",1,A32,A26)</f>
+        <v>ditta:L1DescriptiveDigitalTwin,ditta:SupervisoryDigitalTwin</v>
+      </c>
+      <c r="I37" s="17" t="str">
+        <f t="shared" ref="I37:I41" si="10">I36</f>
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K37" s="17" t="str">
+        <f t="shared" ref="K37:K41" si="11">K36</f>
+        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>ditta:1-DescriptiveDigitalTwin</v>
+      </c>
+      <c r="G38" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>ditta:L2InformativeDigitalTwin,ditta:OperationalDigitalTwin</v>
+      </c>
+      <c r="I38" s="17" t="str">
+        <f t="shared" si="10"/>
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K38" s="17" t="str">
+        <f t="shared" si="11"/>
+        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>ditta:2-DiagnosticDigitalTwin</v>
+      </c>
+      <c r="G39" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>ditta:L3PredictiveDigitalTwin,ditta:Simulation-PredictionDigitalTwin</v>
+      </c>
+      <c r="I39" s="17" t="str">
+        <f t="shared" si="10"/>
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K39" s="17" t="str">
+        <f t="shared" si="11"/>
+        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>ditta:3-PredictiveDigitalTwin</v>
+      </c>
+      <c r="G40" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>ditta:L4LivingDigitalTwin,ditta:Intelligent-LearningDigitalTwin</v>
+      </c>
+      <c r="I40" s="17" t="str">
+        <f t="shared" si="10"/>
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K40" s="17" t="str">
+        <f t="shared" si="11"/>
+        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>ditta:4-PrescriptiveDigitalTwin</v>
+      </c>
+      <c r="F41" s="11" t="str">
+        <f>TEXTJOIN(",",1,A30)</f>
+        <v>ditta:AutonomousDigitalTwin</v>
+      </c>
+      <c r="G41" s="11" t="str">
+        <f>TEXTJOIN(",",1,A31)</f>
+        <v>ditta:CognitiveDigitalTwin</v>
+      </c>
+      <c r="I41" s="17" t="str">
+        <f t="shared" si="10"/>
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K41" s="17" t="str">
+        <f t="shared" si="11"/>
+        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="11" t="str">
+        <f t="shared" ref="A42:A54" si="12">IF(ISBLANK($B42),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B42," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ditta:IntelligentDigitalTwin</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="11" t="str">
+        <f>$A$25</f>
+        <v>ditta:SystemFunctionality</v>
+      </c>
+      <c r="G42" s="11" t="str">
         <f>TEXTJOIN(",",1,A29)</f>
         <v>ditta:Intelligent-LearningDigitalTwin</v>
       </c>
-      <c r="I36" s="14" t="s">
+      <c r="I42" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="14" t="s">
+      <c r="K42" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="11" t="str">
-        <f t="shared" si="1"/>
+    <row r="43">
+      <c r="A43" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:ConnectionSystemAutomation</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="11" t="str">
+      <c r="B43" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="11" t="str">
         <f>$A$18</f>
         <v>ditta:DigitalTwinType</v>
       </c>
-      <c r="H37" s="11" t="str">
+      <c r="H43" s="11" t="str">
         <f>A21</f>
         <v>ditta:ConnectionSystem</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="11" t="str">
-        <f t="shared" si="1"/>
+    <row r="44">
+      <c r="A44" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:ManuallyCoupledDigitalTwin</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="11" t="str">
-        <f t="shared" ref="E38:E40" si="8">A37</f>
+      <c r="B44" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="11" t="str">
+        <f t="shared" ref="E44:E46" si="13">A43</f>
         <v>ditta:ConnectionSystemAutomation</v>
       </c>
-      <c r="I38" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J38" s="14" t="s">
+      <c r="I44" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J44" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K38" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="L38" s="12"/>
-      <c r="N38" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="11" t="str">
-        <f t="shared" si="1"/>
+      <c r="K44" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="L44" s="12"/>
+      <c r="N44" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:DigitalShadow</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E39" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="B45" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="11" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:ManuallyCoupledDigitalTwin</v>
       </c>
-      <c r="I39" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J39" s="14" t="s">
+      <c r="I45" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J45" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K39" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="L39" s="15" t="s">
+      <c r="K45" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="L45" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="N39" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="11" t="str">
-        <f t="shared" si="1"/>
+      <c r="N45" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:FullyCoupledDigitalTwin</v>
       </c>
-      <c r="B40" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E40" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="B46" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="11" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:DigitalShadow</v>
       </c>
-      <c r="I40" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J40" s="14" t="s">
+      <c r="I46" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J46" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="L40" s="15" t="s">
+      <c r="K46" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="L46" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="N40" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="11" t="str">
-        <f t="shared" si="1"/>
+      <c r="N46" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:ModelFidelity</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" s="11" t="str">
+      <c r="B47" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" s="11" t="str">
         <f>$A$18</f>
         <v>ditta:DigitalTwinType</v>
       </c>
-      <c r="H41" s="11" t="str">
+      <c r="H47" s="11" t="str">
         <f>$A$22</f>
         <v>ditta:ModelSystem</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="11" t="str">
-        <f t="shared" si="1"/>
+    <row r="48">
+      <c r="A48" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:LowFidelityDigitalTwin</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E42" s="11" t="str">
-        <f t="shared" ref="E42:E44" si="9">$A$41</f>
+      <c r="B48" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" s="11" t="str">
+        <f t="shared" ref="E48:E50" si="14">$A$47</f>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="11" t="str">
-        <f t="shared" si="1"/>
+    <row r="49">
+      <c r="A49" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:HighFidelityDigitalTwin</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E43" s="11" t="str">
-        <f t="shared" si="9"/>
+      <c r="B49" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E49" s="11" t="str">
+        <f t="shared" si="14"/>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="11" t="str">
-        <f t="shared" si="1"/>
+    <row r="50">
+      <c r="A50" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:Multi-FidelityDigitalTwin</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E44" s="11" t="str">
-        <f t="shared" si="9"/>
+      <c r="B50" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="11" t="str">
+        <f t="shared" si="14"/>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="11" t="str">
-        <f t="shared" si="1"/>
+    <row r="51">
+      <c r="A51" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="11" t="str">
+      <c r="B51" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E51" s="11" t="str">
         <f>$A$18</f>
         <v>ditta:DigitalTwinType</v>
       </c>
-      <c r="H45" s="11" t="str">
+      <c r="H51" s="11" t="str">
         <f>$A$19</f>
         <v>ditta:PhysicalSystem</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="11" t="str">
-        <f t="shared" si="1"/>
+    <row r="52">
+      <c r="A52" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:DigitalTwinPrototype</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="11" t="str">
-        <f t="shared" ref="E46:E48" si="10">$A$45</f>
+      <c r="B52" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" s="11" t="str">
+        <f t="shared" ref="E52:E54" si="15">$A$51</f>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
-      <c r="I46" s="14" t="s">
+      <c r="I52" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K46" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="11" t="str">
-        <f t="shared" si="1"/>
+      <c r="K52" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:DigitalTwinInstance</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E47" s="11" t="str">
-        <f t="shared" si="10"/>
+      <c r="B53" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E53" s="11" t="str">
+        <f t="shared" si="15"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
-      <c r="I47" s="14" t="s">
+      <c r="I53" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K47" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="11" t="str">
-        <f t="shared" si="1"/>
+      <c r="K53" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="11" t="str">
+        <f t="shared" si="12"/>
         <v>ditta:DigitalTwinAggregate</v>
       </c>
-      <c r="B48" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" s="11" t="str">
-        <f t="shared" si="10"/>
+      <c r="B54" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E54" s="11" t="str">
+        <f t="shared" si="15"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
-      <c r="I48" s="14" t="s">
+      <c r="I54" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K48" s="14" t="s">
+      <c r="K54" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1674,24 +1900,26 @@
     <hyperlink r:id="rId23" ref="L31"/>
     <hyperlink r:id="rId24" ref="I36"/>
     <hyperlink r:id="rId25" ref="K36"/>
-    <hyperlink r:id="rId26" ref="I38"/>
-    <hyperlink r:id="rId27" ref="J38"/>
-    <hyperlink r:id="rId28" ref="K38"/>
-    <hyperlink r:id="rId29" ref="I39"/>
-    <hyperlink r:id="rId30" ref="J39"/>
-    <hyperlink r:id="rId31" ref="K39"/>
-    <hyperlink r:id="rId32" ref="L39"/>
-    <hyperlink r:id="rId33" ref="I40"/>
-    <hyperlink r:id="rId34" ref="J40"/>
-    <hyperlink r:id="rId35" ref="K40"/>
-    <hyperlink r:id="rId36" ref="L40"/>
-    <hyperlink r:id="rId37" ref="I46"/>
-    <hyperlink r:id="rId38" ref="K46"/>
-    <hyperlink r:id="rId39" ref="I47"/>
-    <hyperlink r:id="rId40" ref="K47"/>
-    <hyperlink r:id="rId41" ref="I48"/>
-    <hyperlink r:id="rId42" ref="K48"/>
+    <hyperlink r:id="rId26" ref="I42"/>
+    <hyperlink r:id="rId27" ref="K42"/>
+    <hyperlink r:id="rId28" ref="I44"/>
+    <hyperlink r:id="rId29" ref="J44"/>
+    <hyperlink r:id="rId30" ref="K44"/>
+    <hyperlink r:id="rId31" ref="I45"/>
+    <hyperlink r:id="rId32" ref="J45"/>
+    <hyperlink r:id="rId33" ref="K45"/>
+    <hyperlink r:id="rId34" ref="L45"/>
+    <hyperlink r:id="rId35" ref="I46"/>
+    <hyperlink r:id="rId36" ref="J46"/>
+    <hyperlink r:id="rId37" ref="K46"/>
+    <hyperlink r:id="rId38" ref="L46"/>
+    <hyperlink r:id="rId39" ref="I52"/>
+    <hyperlink r:id="rId40" ref="K52"/>
+    <hyperlink r:id="rId41" ref="I53"/>
+    <hyperlink r:id="rId42" ref="K53"/>
+    <hyperlink r:id="rId43" ref="I54"/>
+    <hyperlink r:id="rId44" ref="K54"/>
   </hyperlinks>
-  <drawing r:id="rId43"/>
+  <drawing r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added closeMatch to Standalone twin
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1438,6 +1438,10 @@
         <f>$A$25</f>
         <v>ditta:SystemFunctionality</v>
       </c>
+      <c r="G36" s="11" t="str">
+        <f>A52</f>
+        <v>ditta:DigitalTwinPrototype</v>
+      </c>
       <c r="I36" s="14" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Added closeMatch in functional classifications
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -726,7 +726,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="29.88"/>
     <col customWidth="1" min="2" max="2" width="40.0"/>
-    <col customWidth="1" min="3" max="3" width="43.88"/>
+    <col customWidth="1" min="3" max="3" width="54.88"/>
     <col customWidth="1" min="5" max="5" width="29.5"/>
     <col customWidth="1" min="7" max="7" width="67.75"/>
     <col customWidth="1" min="9" max="9" width="30.5"/>
@@ -1226,6 +1226,10 @@
         <f>$A$25</f>
         <v>ditta:SystemFunctionality</v>
       </c>
+      <c r="G26" s="11" t="str">
+        <f t="shared" ref="G26:G28" si="4">TEXTJOIN(",",1,A32,A37)</f>
+        <v>ditta:L1DescriptiveDigitalTwin,ditta:1-DescriptiveDigitalTwin</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="11" t="str">
@@ -1236,8 +1240,12 @@
         <v>54</v>
       </c>
       <c r="E27" s="11" t="str">
-        <f t="shared" ref="E27:E30" si="4">$A26</f>
+        <f t="shared" ref="E27:E30" si="5">$A26</f>
         <v>ditta:SupervisoryDigitalTwin</v>
+      </c>
+      <c r="G27" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>ditta:L2InformativeDigitalTwin,ditta:2-DiagnosticDigitalTwin</v>
       </c>
       <c r="I27" s="14" t="s">
         <v>55</v>
@@ -1255,8 +1263,12 @@
         <v>57</v>
       </c>
       <c r="E28" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>ditta:OperationalDigitalTwin</v>
+      </c>
+      <c r="G28" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>ditta:OperationalDigitalTwin</v>
+        <v>ditta:L3PredictiveDigitalTwin,ditta:3-PredictiveDigitalTwin</v>
       </c>
       <c r="I28" s="14" t="s">
         <v>55</v>
@@ -1277,8 +1289,12 @@
         <v>59</v>
       </c>
       <c r="E29" s="11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ditta:Simulation-PredictionDigitalTwin</v>
+      </c>
+      <c r="G29" s="11" t="str">
+        <f>TEXTJOIN(",",1,A35,A40,A42)</f>
+        <v>ditta:L4LivingDigitalTwin,ditta:4-PrescriptiveDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
       <c r="I29" s="14" t="s">
         <v>55</v>
@@ -1296,7 +1312,7 @@
         <v>60</v>
       </c>
       <c r="E30" s="11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ditta:Intelligent-LearningDigitalTwin</v>
       </c>
       <c r="F30" s="11" t="str">
@@ -1304,8 +1320,8 @@
         <v>ditta:5-AutonomousDigitalTwin</v>
       </c>
       <c r="G30" s="11" t="str">
-        <f>TEXTJOIN(",",1,A31)</f>
-        <v>ditta:CognitiveDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A31,A35, A42)</f>
+        <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
       <c r="I30" s="14" t="s">
         <v>55</v>
@@ -1322,11 +1338,11 @@
       <c r="B31" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="13" t="s">
         <v>62</v>
       </c>
       <c r="E31" s="11" t="str">
-        <f t="shared" ref="E31:E32" si="5">$A$25</f>
+        <f t="shared" ref="E31:E32" si="6">$A$25</f>
         <v>ditta:SystemFunctionality</v>
       </c>
       <c r="G31" s="11" t="str">
@@ -1352,15 +1368,15 @@
       <c r="B32" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="13" t="s">
         <v>67</v>
       </c>
       <c r="E32" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ditta:SystemFunctionality</v>
       </c>
       <c r="G32" s="11" t="str">
-        <f t="shared" ref="G32:G34" si="6">A26</f>
+        <f t="shared" ref="G32:G34" si="7">A26</f>
         <v>ditta:SupervisoryDigitalTwin</v>
       </c>
     </row>
@@ -1372,15 +1388,15 @@
       <c r="B33" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>69</v>
       </c>
       <c r="E33" s="11" t="str">
-        <f t="shared" ref="E33:E35" si="7">$A32</f>
+        <f t="shared" ref="E33:E35" si="8">$A32</f>
         <v>ditta:L1DescriptiveDigitalTwin</v>
       </c>
       <c r="G33" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>ditta:OperationalDigitalTwin</v>
       </c>
     </row>
@@ -1392,15 +1408,15 @@
       <c r="B34" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="13" t="s">
         <v>71</v>
       </c>
       <c r="E34" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>ditta:L2InformativeDigitalTwin</v>
+      </c>
+      <c r="G34" s="11" t="str">
         <f t="shared" si="7"/>
-        <v>ditta:L2InformativeDigitalTwin</v>
-      </c>
-      <c r="G34" s="11" t="str">
-        <f t="shared" si="6"/>
         <v>ditta:Simulation-PredictionDigitalTwin</v>
       </c>
     </row>
@@ -1412,16 +1428,16 @@
       <c r="B35" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>73</v>
       </c>
       <c r="E35" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>ditta:L3PredictiveDigitalTwin</v>
       </c>
       <c r="G35" s="11" t="str">
-        <f>TEXTJOIN(",",1,A29,A30,A31)</f>
-        <v>ditta:Intelligent-LearningDigitalTwin,ditta:AutonomousDigitalTwin,ditta:CognitiveDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A29,A30,A31,A41,A42)</f>
+        <v>ditta:Intelligent-LearningDigitalTwin,ditta:AutonomousDigitalTwin,ditta:CognitiveDigitalTwin,ditta:5-AutonomousDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
     </row>
     <row r="36">
@@ -1460,19 +1476,19 @@
         <v>81</v>
       </c>
       <c r="E37" s="11" t="str">
-        <f t="shared" ref="E37:E41" si="8">A36</f>
+        <f t="shared" ref="E37:E41" si="9">A36</f>
         <v>ditta:0-StandaloneDigitalTwin</v>
       </c>
       <c r="G37" s="11" t="str">
-        <f t="shared" ref="G37:G40" si="9">TEXTJOIN(",",1,A32,A26)</f>
+        <f t="shared" ref="G37:G39" si="10">TEXTJOIN(",",1,A32,A26)</f>
         <v>ditta:L1DescriptiveDigitalTwin,ditta:SupervisoryDigitalTwin</v>
       </c>
       <c r="I37" s="17" t="str">
-        <f t="shared" ref="I37:I41" si="10">I36</f>
+        <f t="shared" ref="I37:I41" si="11">I36</f>
         <v>https://orcid.org/0009-0003-5155-0870</v>
       </c>
       <c r="K37" s="17" t="str">
-        <f t="shared" ref="K37:K41" si="11">K36</f>
+        <f t="shared" ref="K37:K41" si="12">K36</f>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
@@ -1487,19 +1503,19 @@
         <v>84</v>
       </c>
       <c r="E38" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ditta:1-DescriptiveDigitalTwin</v>
       </c>
       <c r="G38" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>ditta:L2InformativeDigitalTwin,ditta:OperationalDigitalTwin</v>
       </c>
       <c r="I38" s="17" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>https://orcid.org/0009-0003-5155-0870</v>
       </c>
       <c r="K38" s="17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
@@ -1514,19 +1530,19 @@
         <v>87</v>
       </c>
       <c r="E39" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ditta:2-DiagnosticDigitalTwin</v>
       </c>
       <c r="G39" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>ditta:L3PredictiveDigitalTwin,ditta:Simulation-PredictionDigitalTwin</v>
       </c>
       <c r="I39" s="17" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>https://orcid.org/0009-0003-5155-0870</v>
       </c>
       <c r="K39" s="17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
@@ -1541,19 +1557,19 @@
         <v>90</v>
       </c>
       <c r="E40" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ditta:3-PredictiveDigitalTwin</v>
       </c>
       <c r="G40" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v>ditta:L4LivingDigitalTwin,ditta:Intelligent-LearningDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A35,A29, A42)</f>
+        <v>ditta:L4LivingDigitalTwin,ditta:Intelligent-LearningDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
       <c r="I40" s="17" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>https://orcid.org/0009-0003-5155-0870</v>
       </c>
       <c r="K40" s="17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
@@ -1568,7 +1584,7 @@
         <v>92</v>
       </c>
       <c r="E41" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ditta:4-PrescriptiveDigitalTwin</v>
       </c>
       <c r="F41" s="11" t="str">
@@ -1576,21 +1592,21 @@
         <v>ditta:AutonomousDigitalTwin</v>
       </c>
       <c r="G41" s="11" t="str">
-        <f>TEXTJOIN(",",1,A31)</f>
-        <v>ditta:CognitiveDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A31,A35,A42)</f>
+        <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
       <c r="I41" s="17" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>https://orcid.org/0009-0003-5155-0870</v>
       </c>
       <c r="K41" s="17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="11" t="str">
-        <f t="shared" ref="A42:A54" si="12">IF(ISBLANK($B42),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B42," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" ref="A42:A54" si="13">IF(ISBLANK($B42),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B42," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>ditta:IntelligentDigitalTwin</v>
       </c>
       <c r="B42" s="12" t="s">
@@ -1605,8 +1621,8 @@
         <v>ditta:SystemFunctionality</v>
       </c>
       <c r="G42" s="11" t="str">
-        <f>TEXTJOIN(",",1,A29)</f>
-        <v>ditta:Intelligent-LearningDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A29,A41,A40,A35,A30)</f>
+        <v>ditta:Intelligent-LearningDigitalTwin,ditta:5-AutonomousDigitalTwin,ditta:4-PrescriptiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:AutonomousDigitalTwin</v>
       </c>
       <c r="I42" s="14" t="s">
         <v>37</v>
@@ -1617,7 +1633,7 @@
     </row>
     <row r="43">
       <c r="A43" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:ConnectionSystemAutomation</v>
       </c>
       <c r="B43" s="12" t="s">
@@ -1640,7 +1656,7 @@
     </row>
     <row r="44">
       <c r="A44" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:ManuallyCoupledDigitalTwin</v>
       </c>
       <c r="B44" s="12" t="s">
@@ -1653,7 +1669,7 @@
         <v>100</v>
       </c>
       <c r="E44" s="11" t="str">
-        <f t="shared" ref="E44:E46" si="13">A43</f>
+        <f t="shared" ref="E44:E46" si="14">A43</f>
         <v>ditta:ConnectionSystemAutomation</v>
       </c>
       <c r="I44" s="15" t="s">
@@ -1672,7 +1688,7 @@
     </row>
     <row r="45">
       <c r="A45" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:DigitalShadow</v>
       </c>
       <c r="B45" s="12" t="s">
@@ -1685,7 +1701,7 @@
         <v>104</v>
       </c>
       <c r="E45" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>ditta:ManuallyCoupledDigitalTwin</v>
       </c>
       <c r="I45" s="15" t="s">
@@ -1706,7 +1722,7 @@
     </row>
     <row r="46">
       <c r="A46" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:FullyCoupledDigitalTwin</v>
       </c>
       <c r="B46" s="12" t="s">
@@ -1719,7 +1735,7 @@
         <v>109</v>
       </c>
       <c r="E46" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>ditta:DigitalShadow</v>
       </c>
       <c r="I46" s="15" t="s">
@@ -1740,7 +1756,7 @@
     </row>
     <row r="47">
       <c r="A47" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:ModelFidelity</v>
       </c>
       <c r="B47" s="12" t="s">
@@ -1757,46 +1773,46 @@
     </row>
     <row r="48">
       <c r="A48" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:LowFidelityDigitalTwin</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>112</v>
       </c>
       <c r="E48" s="11" t="str">
-        <f t="shared" ref="E48:E50" si="14">$A$47</f>
+        <f t="shared" ref="E48:E50" si="15">$A$47</f>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:HighFidelityDigitalTwin</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>113</v>
       </c>
       <c r="E49" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:Multi-FidelityDigitalTwin</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>114</v>
       </c>
       <c r="E50" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
       <c r="B51" s="12" t="s">
@@ -1813,7 +1829,7 @@
     </row>
     <row r="52">
       <c r="A52" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:DigitalTwinPrototype</v>
       </c>
       <c r="B52" s="12" t="s">
@@ -1823,7 +1839,7 @@
         <v>117</v>
       </c>
       <c r="E52" s="11" t="str">
-        <f t="shared" ref="E52:E54" si="15">$A$51</f>
+        <f t="shared" ref="E52:E54" si="16">$A$51</f>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
       <c r="I52" s="14" t="s">
@@ -1835,7 +1851,7 @@
     </row>
     <row r="53">
       <c r="A53" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:DigitalTwinInstance</v>
       </c>
       <c r="B53" s="12" t="s">
@@ -1845,7 +1861,7 @@
         <v>120</v>
       </c>
       <c r="E53" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
       <c r="I53" s="14" t="s">
@@ -1857,7 +1873,7 @@
     </row>
     <row r="54">
       <c r="A54" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>ditta:DigitalTwinAggregate</v>
       </c>
       <c r="B54" s="12" t="s">
@@ -1867,7 +1883,7 @@
         <v>122</v>
       </c>
       <c r="E54" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
       <c r="I54" s="14" t="s">

</xml_diff>

<commit_message>
Remove DT system concept
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="122">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -64,7 +64,7 @@
     <t>pav:version</t>
   </si>
   <si>
-    <t>0.0.2</t>
+    <t>0.0.3</t>
   </si>
   <si>
     <t>pav:createdOn</t>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>https://doi.org/10.12688/digitaltwin.17574.1</t>
-  </si>
-  <si>
-    <t>Digital Twin System</t>
   </si>
   <si>
     <t>Digital Twin Type</t>
@@ -1058,7 +1055,7 @@
     </row>
     <row r="16">
       <c r="A16" s="11" t="str">
-        <f t="shared" ref="A16:A35" si="1">IF(ISBLANK($B16),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B16," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" ref="A16:A34" si="1">IF(ISBLANK($B16),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B16," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>ditta:DigitalTwinConceptualModel</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -1080,39 +1077,48 @@
     <row r="17">
       <c r="A17" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:DigitalTwinSystem</v>
+        <v>ditta:DigitalTwinType</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="16"/>
+      <c r="I17" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:DigitalTwinType</v>
+        <v>ditta:PhysicalSystem</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>40</v>
       </c>
+      <c r="D18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="11" t="str">
+        <f>A16</f>
+        <v>ditta:DigitalTwinConceptualModel</v>
+      </c>
       <c r="I18" s="14" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:PhysicalSystem</v>
+        <v>ditta:DigitalSystem</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="11" t="str">
-        <f t="shared" ref="E19:E21" si="2">$A$17</f>
-        <v>ditta:DigitalTwinSystem</v>
+        <f>A16</f>
+        <v>ditta:DigitalTwinConceptualModel</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>37</v>
@@ -1121,17 +1127,17 @@
     <row r="20">
       <c r="A20" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:DigitalSystem</v>
+        <v>ditta:ConnectionSystem</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E20" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>ditta:DigitalTwinSystem</v>
+        <f>A16</f>
+        <v>ditta:DigitalTwinConceptualModel</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>37</v>
@@ -1140,756 +1146,737 @@
     <row r="21">
       <c r="A21" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:ConnectionSystem</v>
+        <v>ditta:ModelSystem</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>ditta:DigitalTwinSystem</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>37</v>
+        <f t="shared" ref="E21:E23" si="2">$A$19</f>
+        <v>ditta:DigitalSystem</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:ModelSystem</v>
+        <v>ditta:ServiceSystem</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E22" s="11" t="str">
-        <f t="shared" ref="E22:E24" si="3">$A$20</f>
+        <f t="shared" si="2"/>
         <v>ditta:DigitalSystem</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:ServiceSystem</v>
+        <v>ditta:DataSystem</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>ditta:DigitalSystem</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:DataSystem</v>
+        <v>ditta:SystemFunctionality</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>50</v>
       </c>
+      <c r="C24" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="E24" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>ditta:DigitalSystem</v>
+        <f>$A$17</f>
+        <v>ditta:DigitalTwinType</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="11" t="str">
         <f t="shared" si="1"/>
+        <v>ditta:SupervisoryDigitalTwin</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="11" t="str">
+        <f>$A$24</f>
         <v>ditta:SystemFunctionality</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="11" t="str">
-        <f>$A$18</f>
-        <v>ditta:DigitalTwinType</v>
+      <c r="G25" s="11" t="str">
+        <f t="shared" ref="G25:G27" si="3">TEXTJOIN(",",1,A31,A36)</f>
+        <v>ditta:L1DescriptiveDigitalTwin,ditta:1-DescriptiveDigitalTwin</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:SupervisoryDigitalTwin</v>
+        <v>ditta:OperationalDigitalTwin</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E26" s="11" t="str">
-        <f>$A$25</f>
-        <v>ditta:SystemFunctionality</v>
+        <f t="shared" ref="E26:E29" si="4">$A25</f>
+        <v>ditta:SupervisoryDigitalTwin</v>
       </c>
       <c r="G26" s="11" t="str">
-        <f t="shared" ref="G26:G28" si="4">TEXTJOIN(",",1,A32,A37)</f>
-        <v>ditta:L1DescriptiveDigitalTwin,ditta:1-DescriptiveDigitalTwin</v>
+        <f t="shared" si="3"/>
+        <v>ditta:L2InformativeDigitalTwin,ditta:2-DiagnosticDigitalTwin</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="11" t="str">
         <f t="shared" si="1"/>
+        <v>ditta:Simulation-PredictionDigitalTwin</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="11" t="str">
+        <f t="shared" si="4"/>
         <v>ditta:OperationalDigitalTwin</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="G27" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>ditta:L3PredictiveDigitalTwin,ditta:3-PredictiveDigitalTwin</v>
+      </c>
+      <c r="I27" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="11" t="str">
-        <f t="shared" ref="E27:E30" si="5">$A26</f>
-        <v>ditta:SupervisoryDigitalTwin</v>
-      </c>
-      <c r="G27" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>ditta:L2InformativeDigitalTwin,ditta:2-DiagnosticDigitalTwin</v>
-      </c>
-      <c r="I27" s="14" t="s">
+      <c r="K27" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:Simulation-PredictionDigitalTwin</v>
+        <v>ditta:Intelligent-LearningDigitalTwin</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>57</v>
       </c>
+      <c r="D28" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="E28" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>ditta:OperationalDigitalTwin</v>
+        <f t="shared" si="4"/>
+        <v>ditta:Simulation-PredictionDigitalTwin</v>
       </c>
       <c r="G28" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>ditta:L3PredictiveDigitalTwin,ditta:3-PredictiveDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A34,A39,A41)</f>
+        <v>ditta:L4LivingDigitalTwin,ditta:4-PrescriptiveDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
       <c r="I28" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="11" t="str">
         <f t="shared" si="1"/>
+        <v>ditta:AutonomousDigitalTwin</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="11" t="str">
+        <f t="shared" si="4"/>
         <v>ditta:Intelligent-LearningDigitalTwin</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>ditta:Simulation-PredictionDigitalTwin</v>
+      <c r="F29" s="11" t="str">
+        <f>TEXTJOIN(",",1,A40)</f>
+        <v>ditta:5-AutonomousDigitalTwin</v>
       </c>
       <c r="G29" s="11" t="str">
-        <f>TEXTJOIN(",",1,A35,A40,A42)</f>
-        <v>ditta:L4LivingDigitalTwin,ditta:4-PrescriptiveDigitalTwin,ditta:IntelligentDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A30,A34, A41)</f>
+        <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
       <c r="I29" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="K29" s="14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:AutonomousDigitalTwin</v>
+        <v>ditta:CognitiveDigitalTwin</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>60</v>
       </c>
+      <c r="C30" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="E30" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v>ditta:Intelligent-LearningDigitalTwin</v>
-      </c>
-      <c r="F30" s="11" t="str">
-        <f>TEXTJOIN(",",1,A41)</f>
-        <v>ditta:5-AutonomousDigitalTwin</v>
+        <f t="shared" ref="E30:E31" si="5">$A$24</f>
+        <v>ditta:SystemFunctionality</v>
       </c>
       <c r="G30" s="11" t="str">
-        <f>TEXTJOIN(",",1,A31,A35, A42)</f>
-        <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:IntelligentDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A29,A34)</f>
+        <v>ditta:AutonomousDigitalTwin,ditta:L4LivingDigitalTwin</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="J30" s="16"/>
+      <c r="K30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L30" s="15" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>ditta:CognitiveDigitalTwin</v>
+        <v>ditta:L1DescriptiveDigitalTwin</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E31" s="11" t="str">
-        <f t="shared" ref="E31:E32" si="6">$A$25</f>
+        <f t="shared" si="5"/>
         <v>ditta:SystemFunctionality</v>
       </c>
       <c r="G31" s="11" t="str">
-        <f>TEXTJOIN(",",1,A30,A35)</f>
-        <v>ditta:AutonomousDigitalTwin,ditta:L4LivingDigitalTwin</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="L31" s="15" t="s">
-        <v>65</v>
+        <f t="shared" ref="G31:G33" si="6">A25</f>
+        <v>ditta:SupervisoryDigitalTwin</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="11" t="str">
         <f t="shared" si="1"/>
+        <v>ditta:L2InformativeDigitalTwin</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="11" t="str">
+        <f t="shared" ref="E32:E34" si="7">$A31</f>
         <v>ditta:L1DescriptiveDigitalTwin</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="11" t="str">
+      <c r="G32" s="11" t="str">
         <f t="shared" si="6"/>
-        <v>ditta:SystemFunctionality</v>
-      </c>
-      <c r="G32" s="11" t="str">
-        <f t="shared" ref="G32:G34" si="7">A26</f>
-        <v>ditta:SupervisoryDigitalTwin</v>
+        <v>ditta:OperationalDigitalTwin</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="11" t="str">
         <f t="shared" si="1"/>
+        <v>ditta:L3PredictiveDigitalTwin</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>ditta:L2InformativeDigitalTwin</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="11" t="str">
-        <f t="shared" ref="E33:E35" si="8">$A32</f>
-        <v>ditta:L1DescriptiveDigitalTwin</v>
-      </c>
       <c r="G33" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v>ditta:OperationalDigitalTwin</v>
+        <f t="shared" si="6"/>
+        <v>ditta:Simulation-PredictionDigitalTwin</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="11" t="str">
         <f t="shared" si="1"/>
+        <v>ditta:L4LivingDigitalTwin</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>ditta:L3PredictiveDigitalTwin</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v>ditta:L2InformativeDigitalTwin</v>
-      </c>
       <c r="G34" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v>ditta:Simulation-PredictionDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A28,A29,A30,A40,A41)</f>
+        <v>ditta:Intelligent-LearningDigitalTwin,ditta:AutonomousDigitalTwin,ditta:CognitiveDigitalTwin,ditta:5-AutonomousDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>ditta:L4LivingDigitalTwin</v>
+      <c r="A35" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E35" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v>ditta:L3PredictiveDigitalTwin</v>
+        <f>$A$24</f>
+        <v>ditta:SystemFunctionality</v>
       </c>
       <c r="G35" s="11" t="str">
-        <f>TEXTJOIN(",",1,A29,A30,A31,A41,A42)</f>
-        <v>ditta:Intelligent-LearningDigitalTwin,ditta:AutonomousDigitalTwin,ditta:CognitiveDigitalTwin,ditta:5-AutonomousDigitalTwin,ditta:IntelligentDigitalTwin</v>
+        <f>A51</f>
+        <v>ditta:DigitalTwinPrototype</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="12" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E36" s="11" t="str">
-        <f>$A$25</f>
-        <v>ditta:SystemFunctionality</v>
+        <f t="shared" ref="E36:E40" si="8">A35</f>
+        <v>ditta:0-StandaloneDigitalTwin</v>
       </c>
       <c r="G36" s="11" t="str">
-        <f>A52</f>
-        <v>ditta:DigitalTwinPrototype</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="K36" s="14" t="s">
-        <v>78</v>
+        <f t="shared" ref="G36:G38" si="9">TEXTJOIN(",",1,A31,A25)</f>
+        <v>ditta:L1DescriptiveDigitalTwin,ditta:SupervisoryDigitalTwin</v>
+      </c>
+      <c r="I36" s="17" t="str">
+        <f t="shared" ref="I36:I40" si="10">I35</f>
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K36" s="17" t="str">
+        <f t="shared" ref="K36:K40" si="11">K35</f>
+        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E37" s="11" t="str">
-        <f t="shared" ref="E37:E41" si="9">A36</f>
-        <v>ditta:0-StandaloneDigitalTwin</v>
+        <f t="shared" si="8"/>
+        <v>ditta:1-DescriptiveDigitalTwin</v>
       </c>
       <c r="G37" s="11" t="str">
-        <f t="shared" ref="G37:G39" si="10">TEXTJOIN(",",1,A32,A26)</f>
-        <v>ditta:L1DescriptiveDigitalTwin,ditta:SupervisoryDigitalTwin</v>
+        <f t="shared" si="9"/>
+        <v>ditta:L2InformativeDigitalTwin,ditta:OperationalDigitalTwin</v>
       </c>
       <c r="I37" s="17" t="str">
-        <f t="shared" ref="I37:I41" si="11">I36</f>
+        <f t="shared" si="10"/>
         <v>https://orcid.org/0009-0003-5155-0870</v>
       </c>
       <c r="K37" s="17" t="str">
-        <f t="shared" ref="K37:K41" si="12">K36</f>
+        <f t="shared" si="11"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E38" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>ditta:2-DiagnosticDigitalTwin</v>
+      </c>
+      <c r="G38" s="11" t="str">
         <f t="shared" si="9"/>
-        <v>ditta:1-DescriptiveDigitalTwin</v>
-      </c>
-      <c r="G38" s="11" t="str">
+        <v>ditta:L3PredictiveDigitalTwin,ditta:Simulation-PredictionDigitalTwin</v>
+      </c>
+      <c r="I38" s="17" t="str">
         <f t="shared" si="10"/>
-        <v>ditta:L2InformativeDigitalTwin,ditta:OperationalDigitalTwin</v>
-      </c>
-      <c r="I38" s="17" t="str">
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K38" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>https://orcid.org/0009-0003-5155-0870</v>
-      </c>
-      <c r="K38" s="17" t="str">
-        <f t="shared" si="12"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E39" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v>ditta:2-DiagnosticDigitalTwin</v>
+        <f t="shared" si="8"/>
+        <v>ditta:3-PredictiveDigitalTwin</v>
       </c>
       <c r="G39" s="11" t="str">
+        <f>TEXTJOIN(",",1,A34,A28, A41)</f>
+        <v>ditta:L4LivingDigitalTwin,ditta:Intelligent-LearningDigitalTwin,ditta:IntelligentDigitalTwin</v>
+      </c>
+      <c r="I39" s="17" t="str">
         <f t="shared" si="10"/>
-        <v>ditta:L3PredictiveDigitalTwin,ditta:Simulation-PredictionDigitalTwin</v>
-      </c>
-      <c r="I39" s="17" t="str">
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K39" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>https://orcid.org/0009-0003-5155-0870</v>
-      </c>
-      <c r="K39" s="17" t="str">
-        <f t="shared" si="12"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E40" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v>ditta:3-PredictiveDigitalTwin</v>
+        <f t="shared" si="8"/>
+        <v>ditta:4-PrescriptiveDigitalTwin</v>
+      </c>
+      <c r="F40" s="11" t="str">
+        <f>TEXTJOIN(",",1,A29)</f>
+        <v>ditta:AutonomousDigitalTwin</v>
       </c>
       <c r="G40" s="11" t="str">
-        <f>TEXTJOIN(",",1,A35,A29, A42)</f>
-        <v>ditta:L4LivingDigitalTwin,ditta:Intelligent-LearningDigitalTwin,ditta:IntelligentDigitalTwin</v>
+        <f>TEXTJOIN(",",1,A30,A34,A41)</f>
+        <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
       <c r="I40" s="17" t="str">
+        <f t="shared" si="10"/>
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K40" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>https://orcid.org/0009-0003-5155-0870</v>
-      </c>
-      <c r="K40" s="17" t="str">
-        <f t="shared" si="12"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="12" t="s">
-        <v>91</v>
+      <c r="A41" s="11" t="str">
+        <f t="shared" ref="A41:A53" si="12">IF(ISBLANK($B41),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B41," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ditta:IntelligentDigitalTwin</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="13" t="s">
         <v>92</v>
       </c>
+      <c r="C41" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="12"/>
       <c r="E41" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v>ditta:4-PrescriptiveDigitalTwin</v>
-      </c>
-      <c r="F41" s="11" t="str">
-        <f>TEXTJOIN(",",1,A30)</f>
-        <v>ditta:AutonomousDigitalTwin</v>
+        <f>$A$24</f>
+        <v>ditta:SystemFunctionality</v>
       </c>
       <c r="G41" s="11" t="str">
-        <f>TEXTJOIN(",",1,A31,A35,A42)</f>
-        <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:IntelligentDigitalTwin</v>
-      </c>
-      <c r="I41" s="17" t="str">
-        <f t="shared" si="11"/>
-        <v>https://orcid.org/0009-0003-5155-0870</v>
-      </c>
-      <c r="K41" s="17" t="str">
-        <f t="shared" si="12"/>
-        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
+        <f>TEXTJOIN(",",1,A28,A40,A39,A34,A29)</f>
+        <v>ditta:Intelligent-LearningDigitalTwin,ditta:5-AutonomousDigitalTwin,ditta:4-PrescriptiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:AutonomousDigitalTwin</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="11" t="str">
-        <f t="shared" ref="A42:A54" si="13">IF(ISBLANK($B42),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B42," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>ditta:IntelligentDigitalTwin</v>
+        <f t="shared" si="12"/>
+        <v>ditta:ConnectionSystemAutomation</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="12"/>
+        <v>95</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>96</v>
+      </c>
       <c r="E42" s="11" t="str">
-        <f>$A$25</f>
-        <v>ditta:SystemFunctionality</v>
-      </c>
-      <c r="G42" s="11" t="str">
-        <f>TEXTJOIN(",",1,A29,A41,A40,A35,A30)</f>
-        <v>ditta:Intelligent-LearningDigitalTwin,ditta:5-AutonomousDigitalTwin,ditta:4-PrescriptiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:AutonomousDigitalTwin</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K42" s="14" t="s">
-        <v>38</v>
+        <f>$A$17</f>
+        <v>ditta:DigitalTwinType</v>
+      </c>
+      <c r="H42" s="11" t="str">
+        <f>A20</f>
+        <v>ditta:ConnectionSystem</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
+        <v>ditta:ManuallyCoupledDigitalTwin</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E43" s="11" t="str">
+        <f t="shared" ref="E43:E45" si="13">A42</f>
         <v>ditta:ConnectionSystemAutomation</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E43" s="11" t="str">
-        <f>$A$18</f>
-        <v>ditta:DigitalTwinType</v>
-      </c>
-      <c r="H43" s="11" t="str">
-        <f>A21</f>
-        <v>ditta:ConnectionSystem</v>
+      <c r="I43" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K43" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="L43" s="12"/>
+      <c r="N43" s="12" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>ditta:DigitalShadow</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="11" t="str">
         <f t="shared" si="13"/>
         <v>ditta:ManuallyCoupledDigitalTwin</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="12" t="s">
+      <c r="I44" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="E44" s="11" t="str">
-        <f t="shared" ref="E44:E46" si="14">A43</f>
-        <v>ditta:ConnectionSystemAutomation</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>101</v>
       </c>
       <c r="J44" s="14" t="s">
         <v>14</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="L44" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L44" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="N44" s="12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>ditta:FullyCoupledDigitalTwin</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" s="11" t="str">
         <f t="shared" si="13"/>
         <v>ditta:DigitalShadow</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E45" s="11" t="str">
-        <f t="shared" si="14"/>
-        <v>ditta:ManuallyCoupledDigitalTwin</v>
-      </c>
       <c r="I45" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J45" s="14" t="s">
         <v>14</v>
       </c>
       <c r="K45" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L45" s="15" t="s">
         <v>38</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="11" t="str">
-        <f t="shared" si="13"/>
-        <v>ditta:FullyCoupledDigitalTwin</v>
+        <f t="shared" si="12"/>
+        <v>ditta:ModelFidelity</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E46" s="11" t="str">
-        <f t="shared" si="14"/>
-        <v>ditta:DigitalShadow</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="J46" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K46" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="L46" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="N46" s="12" t="s">
-        <v>110</v>
+        <f>$A$17</f>
+        <v>ditta:DigitalTwinType</v>
+      </c>
+      <c r="H46" s="11" t="str">
+        <f>$A$21</f>
+        <v>ditta:ModelSystem</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="11" t="str">
-        <f t="shared" si="13"/>
-        <v>ditta:ModelFidelity</v>
+        <f t="shared" si="12"/>
+        <v>ditta:LowFidelityDigitalTwin</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>111</v>
       </c>
       <c r="E47" s="11" t="str">
-        <f>$A$18</f>
-        <v>ditta:DigitalTwinType</v>
-      </c>
-      <c r="H47" s="11" t="str">
-        <f>$A$22</f>
-        <v>ditta:ModelSystem</v>
+        <f t="shared" ref="E47:E49" si="14">$A$46</f>
+        <v>ditta:ModelFidelity</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="11" t="str">
-        <f t="shared" si="13"/>
-        <v>ditta:LowFidelityDigitalTwin</v>
+        <f t="shared" si="12"/>
+        <v>ditta:HighFidelityDigitalTwin</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>112</v>
       </c>
       <c r="E48" s="11" t="str">
-        <f t="shared" ref="E48:E50" si="15">$A$47</f>
+        <f t="shared" si="14"/>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="11" t="str">
-        <f t="shared" si="13"/>
-        <v>ditta:HighFidelityDigitalTwin</v>
+        <f t="shared" si="12"/>
+        <v>ditta:Multi-FidelityDigitalTwin</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>113</v>
       </c>
       <c r="E49" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="11" t="str">
-        <f t="shared" si="13"/>
-        <v>ditta:Multi-FidelityDigitalTwin</v>
+        <f t="shared" si="12"/>
+        <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>114</v>
       </c>
       <c r="E50" s="11" t="str">
-        <f t="shared" si="15"/>
-        <v>ditta:ModelFidelity</v>
+        <f>$A$17</f>
+        <v>ditta:DigitalTwinType</v>
+      </c>
+      <c r="H50" s="11" t="str">
+        <f>$A$18</f>
+        <v>ditta:PhysicalSystem</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="11" t="str">
-        <f t="shared" si="13"/>
-        <v>ditta:PhysicalSystemLifetimeStage</v>
+        <f t="shared" si="12"/>
+        <v>ditta:DigitalTwinPrototype</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>115</v>
       </c>
+      <c r="C51" s="18" t="s">
+        <v>116</v>
+      </c>
       <c r="E51" s="11" t="str">
-        <f>$A$18</f>
-        <v>ditta:DigitalTwinType</v>
-      </c>
-      <c r="H51" s="11" t="str">
-        <f>$A$19</f>
-        <v>ditta:PhysicalSystem</v>
+        <f t="shared" ref="E51:E53" si="15">$A$50</f>
+        <v>ditta:PhysicalSystemLifetimeStage</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K51" s="14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="11" t="str">
-        <f t="shared" si="13"/>
-        <v>ditta:DigitalTwinPrototype</v>
+        <f t="shared" si="12"/>
+        <v>ditta:DigitalTwinInstance</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="E52" s="11" t="str">
-        <f t="shared" ref="E52:E54" si="16">$A$51</f>
+        <f t="shared" si="15"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
       <c r="I52" s="14" t="s">
         <v>37</v>
       </c>
       <c r="K52" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="11" t="str">
-        <f t="shared" si="13"/>
-        <v>ditta:DigitalTwinInstance</v>
+        <f t="shared" si="12"/>
+        <v>ditta:DigitalTwinAggregate</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E53" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
       <c r="I53" s="14" t="s">
         <v>37</v>
       </c>
       <c r="K53" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="11" t="str">
-        <f t="shared" si="13"/>
-        <v>ditta:DigitalTwinAggregate</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="E54" s="11" t="str">
-        <f t="shared" si="16"/>
-        <v>ditta:PhysicalSystemLifetimeStage</v>
-      </c>
-      <c r="I54" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K54" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1903,42 +1890,42 @@
     <hyperlink r:id="rId6" ref="B9"/>
     <hyperlink r:id="rId7" ref="I16"/>
     <hyperlink r:id="rId8" ref="K16"/>
-    <hyperlink r:id="rId9" ref="I18"/>
-    <hyperlink r:id="rId10" ref="I19"/>
-    <hyperlink r:id="rId11" ref="I20"/>
-    <hyperlink r:id="rId12" ref="I21"/>
-    <hyperlink r:id="rId13" ref="I27"/>
-    <hyperlink r:id="rId14" ref="K27"/>
-    <hyperlink r:id="rId15" ref="I28"/>
-    <hyperlink r:id="rId16" ref="K28"/>
-    <hyperlink r:id="rId17" ref="I29"/>
-    <hyperlink r:id="rId18" ref="K29"/>
-    <hyperlink r:id="rId19" ref="I30"/>
-    <hyperlink r:id="rId20" ref="K30"/>
-    <hyperlink r:id="rId21" ref="I31"/>
-    <hyperlink r:id="rId22" ref="K31"/>
-    <hyperlink r:id="rId23" ref="L31"/>
-    <hyperlink r:id="rId24" ref="I36"/>
-    <hyperlink r:id="rId25" ref="K36"/>
-    <hyperlink r:id="rId26" ref="I42"/>
-    <hyperlink r:id="rId27" ref="K42"/>
-    <hyperlink r:id="rId28" ref="I44"/>
-    <hyperlink r:id="rId29" ref="J44"/>
-    <hyperlink r:id="rId30" ref="K44"/>
-    <hyperlink r:id="rId31" ref="I45"/>
-    <hyperlink r:id="rId32" ref="J45"/>
-    <hyperlink r:id="rId33" ref="K45"/>
-    <hyperlink r:id="rId34" ref="L45"/>
-    <hyperlink r:id="rId35" ref="I46"/>
-    <hyperlink r:id="rId36" ref="J46"/>
-    <hyperlink r:id="rId37" ref="K46"/>
-    <hyperlink r:id="rId38" ref="L46"/>
-    <hyperlink r:id="rId39" ref="I52"/>
-    <hyperlink r:id="rId40" ref="K52"/>
-    <hyperlink r:id="rId41" ref="I53"/>
-    <hyperlink r:id="rId42" ref="K53"/>
-    <hyperlink r:id="rId43" ref="I54"/>
-    <hyperlink r:id="rId44" ref="K54"/>
+    <hyperlink r:id="rId9" ref="I17"/>
+    <hyperlink r:id="rId10" ref="I18"/>
+    <hyperlink r:id="rId11" ref="I19"/>
+    <hyperlink r:id="rId12" ref="I20"/>
+    <hyperlink r:id="rId13" ref="I26"/>
+    <hyperlink r:id="rId14" ref="K26"/>
+    <hyperlink r:id="rId15" ref="I27"/>
+    <hyperlink r:id="rId16" ref="K27"/>
+    <hyperlink r:id="rId17" ref="I28"/>
+    <hyperlink r:id="rId18" ref="K28"/>
+    <hyperlink r:id="rId19" ref="I29"/>
+    <hyperlink r:id="rId20" ref="K29"/>
+    <hyperlink r:id="rId21" ref="I30"/>
+    <hyperlink r:id="rId22" ref="K30"/>
+    <hyperlink r:id="rId23" ref="L30"/>
+    <hyperlink r:id="rId24" ref="I35"/>
+    <hyperlink r:id="rId25" ref="K35"/>
+    <hyperlink r:id="rId26" ref="I41"/>
+    <hyperlink r:id="rId27" ref="K41"/>
+    <hyperlink r:id="rId28" ref="I43"/>
+    <hyperlink r:id="rId29" ref="J43"/>
+    <hyperlink r:id="rId30" ref="K43"/>
+    <hyperlink r:id="rId31" ref="I44"/>
+    <hyperlink r:id="rId32" ref="J44"/>
+    <hyperlink r:id="rId33" ref="K44"/>
+    <hyperlink r:id="rId34" ref="L44"/>
+    <hyperlink r:id="rId35" ref="I45"/>
+    <hyperlink r:id="rId36" ref="J45"/>
+    <hyperlink r:id="rId37" ref="K45"/>
+    <hyperlink r:id="rId38" ref="L45"/>
+    <hyperlink r:id="rId39" ref="I51"/>
+    <hyperlink r:id="rId40" ref="K51"/>
+    <hyperlink r:id="rId41" ref="I52"/>
+    <hyperlink r:id="rId42" ref="K52"/>
+    <hyperlink r:id="rId43" ref="I53"/>
+    <hyperlink r:id="rId44" ref="K53"/>
   </hyperlinks>
   <drawing r:id="rId45"/>
 </worksheet>

</xml_diff>

<commit_message>
Added five-dimensional digital twin definition
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="135">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -25,18 +25,15 @@
     <t>ditta</t>
   </si>
   <si>
-    <t>pav</t>
-  </si>
-  <si>
-    <t>http://purl.org/pav/</t>
-  </si>
-  <si>
     <t>dct</t>
   </si>
   <si>
     <t>http://purl.org/dc/terms/</t>
   </si>
   <si>
+    <t>owl</t>
+  </si>
+  <si>
     <t>skos:prefLabel</t>
   </si>
   <si>
@@ -58,22 +55,28 @@
     <t>https://orcid.org/0000-0002-6570-6966</t>
   </si>
   <si>
+    <t>dct:publisher</t>
+  </si>
+  <si>
+    <t>OST - Ostschweizer Fachhochschule</t>
+  </si>
+  <si>
     <t>dct:contributor</t>
   </si>
   <si>
-    <t>pav:version</t>
-  </si>
-  <si>
-    <t>0.0.3</t>
-  </si>
-  <si>
-    <t>pav:createdOn</t>
-  </si>
-  <si>
-    <t>2020-12-01T00:00:00+01:00</t>
-  </si>
-  <si>
-    <t>pav:lastUpdatedOn</t>
+    <t>dct:license</t>
+  </si>
+  <si>
+    <t>http://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
+    <t>owl:versionInfo</t>
+  </si>
+  <si>
+    <t>0.0.4</t>
+  </si>
+  <si>
+    <t>dct:hasVersion</t>
   </si>
   <si>
     <t>Identifier</t>
@@ -157,12 +160,36 @@
     <t>Virtual Entity</t>
   </si>
   <si>
+    <t>https://orcid.org/0000-0002-9020-0633</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/B978-0-12-817630-6.00003-5</t>
+  </si>
+  <si>
+    <t>Tao et al. (2019) refer to this concept as Virtual Entity and consider this system to be on the same hierarchical level as physical system and connection system.</t>
+  </si>
+  <si>
     <t>Service System</t>
   </si>
   <si>
+    <t>Tao et al. (2019) consider this system to be on the same hierarchical level as physical system and connection system.</t>
+  </si>
+  <si>
     <t>Data System</t>
   </si>
   <si>
+    <t>Geometry Model</t>
+  </si>
+  <si>
+    <t>Physics Model</t>
+  </si>
+  <si>
+    <t>Behaviour Model</t>
+  </si>
+  <si>
+    <t>Rule Model</t>
+  </si>
+  <si>
     <t>System Functionality</t>
   </si>
   <si>
@@ -377,13 +404,25 @@
   </si>
   <si>
     <t>Digital Twin Aggregate, the aggregation of all the DTIs or all the products that have been built.</t>
+  </si>
+  <si>
+    <t>Conceptual Model Dimensionality</t>
+  </si>
+  <si>
+    <t>Three-dimensional Digital Twin</t>
+  </si>
+  <si>
+    <t>Five-dimensional Digital Twin</t>
+  </si>
+  <si>
+    <t>A five-dimensional digital twin destinguishes between models, data, and service concepts instead of a single term for a digital representation in the Digital Twin Conceptual Model.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -415,9 +454,18 @@
       <name val="Helvetica"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
       <u/>
       <color rgb="FF0000FF"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
@@ -451,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -476,33 +524,39 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -799,12 +853,10 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -819,10 +871,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -839,10 +891,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -859,10 +911,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -879,10 +931,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -898,11 +950,11 @@
       <c r="N8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -921,8 +973,8 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
+      <c r="B10" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -938,11 +990,11 @@
       <c r="N10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -958,11 +1010,11 @@
       <c r="N11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -978,8 +1030,13 @@
       <c r="N12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f>B12</f>
+        <v>0.0.4</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1011,873 +1068,1032 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="G15" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="H15" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="I15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="K15" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="L15" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="M15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="str">
-        <f t="shared" ref="A16:A34" si="1">IF(ISBLANK($B16),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B16," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+      <c r="A16" s="13" t="str">
+        <f t="shared" ref="A16:A38" si="1">IF(ISBLANK($B16),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B16," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>ditta:DigitalTwinConceptualModel</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="D16" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="I16" s="16" t="s">
         <v>38</v>
       </c>
+      <c r="K16" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="str">
+      <c r="A17" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:DigitalTwinType</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>14</v>
+      <c r="B17" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="str">
+      <c r="A18" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:PhysicalSystem</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="B18" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="11" t="str">
+      <c r="D18" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="13" t="str">
         <f>A16</f>
         <v>ditta:DigitalTwinConceptualModel</v>
       </c>
-      <c r="I18" s="14" t="s">
-        <v>37</v>
+      <c r="I18" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="str">
+      <c r="A19" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:DigitalSystem</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="B19" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="11" t="str">
+      <c r="D19" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="13" t="str">
         <f>A16</f>
         <v>ditta:DigitalTwinConceptualModel</v>
       </c>
-      <c r="I19" s="14" t="s">
-        <v>37</v>
+      <c r="I19" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11" t="str">
+      <c r="A20" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:ConnectionSystem</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="B20" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="11" t="str">
+      <c r="D20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="13" t="str">
         <f>A16</f>
         <v>ditta:DigitalTwinConceptualModel</v>
       </c>
-      <c r="I20" s="14" t="s">
-        <v>37</v>
+      <c r="I20" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11" t="str">
+      <c r="A21" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:ModelSystem</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="B21" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="11" t="str">
+      <c r="D21" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="13" t="str">
         <f t="shared" ref="E21:E23" si="2">$A$19</f>
         <v>ditta:DigitalSystem</v>
       </c>
+      <c r="I21" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="11" t="str">
+      <c r="A22" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:ServiceSystem</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="11" t="str">
+      <c r="B22" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="13" t="str">
         <f t="shared" si="2"/>
         <v>ditta:DigitalSystem</v>
       </c>
+      <c r="I22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="11" t="str">
+      <c r="A23" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:DataSystem</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="11" t="str">
+      <c r="B23" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="13" t="str">
         <f t="shared" si="2"/>
         <v>ditta:DigitalSystem</v>
       </c>
+      <c r="I23" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="11" t="str">
+      <c r="A24" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>ditta:GeometryModel</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="E24" s="13" t="str">
+        <f t="shared" ref="E24:E27" si="3">$A$21</f>
+        <v>ditta:ModelSystem</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>ditta:PhysicsModel</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="E25" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>ditta:ModelSystem</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>ditta:BehaviourModel</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="E26" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>ditta:ModelSystem</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>ditta:RuleModel</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="E27" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>ditta:ModelSystem</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:SystemFunctionality</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="11" t="str">
+      <c r="B28" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="13" t="str">
         <f>$A$17</f>
         <v>ditta:DigitalTwinType</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="11" t="str">
+    <row r="29">
+      <c r="A29" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:SupervisoryDigitalTwin</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="11" t="str">
-        <f>$A$24</f>
+      <c r="B29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="13" t="str">
+        <f>$A$28</f>
         <v>ditta:SystemFunctionality</v>
       </c>
-      <c r="G25" s="11" t="str">
-        <f t="shared" ref="G25:G27" si="3">TEXTJOIN(",",1,A31,A36)</f>
+      <c r="G29" s="13" t="str">
+        <f t="shared" ref="G29:G31" si="4">TEXTJOIN(",",1,A35,A40)</f>
         <v>ditta:L1DescriptiveDigitalTwin,ditta:1-DescriptiveDigitalTwin</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="11" t="str">
+    <row r="30">
+      <c r="A30" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:OperationalDigitalTwin</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="11" t="str">
-        <f t="shared" ref="E26:E29" si="4">$A25</f>
+      <c r="B30" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="13" t="str">
+        <f t="shared" ref="E30:E33" si="5">$A29</f>
         <v>ditta:SupervisoryDigitalTwin</v>
       </c>
-      <c r="G26" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="G30" s="13" t="str">
+        <f t="shared" si="4"/>
         <v>ditta:L2InformativeDigitalTwin,ditta:2-DiagnosticDigitalTwin</v>
       </c>
-      <c r="I26" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="11" t="str">
+      <c r="I30" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:Simulation-PredictionDigitalTwin</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="11" t="str">
+      <c r="B31" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>ditta:OperationalDigitalTwin</v>
+      </c>
+      <c r="G31" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>ditta:OperationalDigitalTwin</v>
-      </c>
-      <c r="G27" s="11" t="str">
-        <f t="shared" si="3"/>
         <v>ditta:L3PredictiveDigitalTwin,ditta:3-PredictiveDigitalTwin</v>
       </c>
-      <c r="I27" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="11" t="str">
+      <c r="I31" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:Intelligent-LearningDigitalTwin</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="11" t="str">
-        <f t="shared" si="4"/>
+      <c r="B32" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="13" t="str">
+        <f t="shared" si="5"/>
         <v>ditta:Simulation-PredictionDigitalTwin</v>
       </c>
-      <c r="G28" s="11" t="str">
-        <f>TEXTJOIN(",",1,A34,A39,A41)</f>
+      <c r="G32" s="13" t="str">
+        <f>TEXTJOIN(",",1,A38,A43,A45)</f>
         <v>ditta:L4LivingDigitalTwin,ditta:4-PrescriptiveDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
-      <c r="I28" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="11" t="str">
+      <c r="I32" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K32" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:AutonomousDigitalTwin</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="11" t="str">
-        <f t="shared" si="4"/>
+      <c r="B33" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="13" t="str">
+        <f t="shared" si="5"/>
         <v>ditta:Intelligent-LearningDigitalTwin</v>
       </c>
-      <c r="F29" s="11" t="str">
-        <f>TEXTJOIN(",",1,A40)</f>
+      <c r="F33" s="13" t="str">
+        <f>TEXTJOIN(",",1,A44)</f>
         <v>ditta:5-AutonomousDigitalTwin</v>
       </c>
-      <c r="G29" s="11" t="str">
-        <f>TEXTJOIN(",",1,A30,A34, A41)</f>
+      <c r="G33" s="13" t="str">
+        <f>TEXTJOIN(",",1,A34,A38, A45)</f>
         <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
-      <c r="I29" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K29" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="11" t="str">
+      <c r="I33" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:CognitiveDigitalTwin</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="11" t="str">
-        <f t="shared" ref="E30:E31" si="5">$A$24</f>
+      <c r="B34" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="13" t="str">
+        <f t="shared" ref="E34:E35" si="6">$A$28</f>
         <v>ditta:SystemFunctionality</v>
       </c>
-      <c r="G30" s="11" t="str">
-        <f>TEXTJOIN(",",1,A29,A34)</f>
+      <c r="G34" s="13" t="str">
+        <f>TEXTJOIN(",",1,A33,A38)</f>
         <v>ditta:AutonomousDigitalTwin,ditta:L4LivingDigitalTwin</v>
       </c>
-      <c r="I30" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="J30" s="16"/>
-      <c r="K30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L30" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="11" t="str">
+      <c r="I34" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J34" s="18"/>
+      <c r="K34" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:L1DescriptiveDigitalTwin</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="11" t="str">
-        <f t="shared" si="5"/>
+      <c r="B35" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="13" t="str">
+        <f t="shared" si="6"/>
         <v>ditta:SystemFunctionality</v>
       </c>
-      <c r="G31" s="11" t="str">
-        <f t="shared" ref="G31:G33" si="6">A25</f>
+      <c r="G35" s="13" t="str">
+        <f t="shared" ref="G35:G37" si="7">A29</f>
         <v>ditta:SupervisoryDigitalTwin</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="11" t="str">
+    <row r="36">
+      <c r="A36" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:L2InformativeDigitalTwin</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="11" t="str">
-        <f t="shared" ref="E32:E34" si="7">$A31</f>
+      <c r="B36" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="13" t="str">
+        <f t="shared" ref="E36:E38" si="8">$A35</f>
         <v>ditta:L1DescriptiveDigitalTwin</v>
       </c>
-      <c r="G32" s="11" t="str">
-        <f t="shared" si="6"/>
+      <c r="G36" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>ditta:OperationalDigitalTwin</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="11" t="str">
+    <row r="37">
+      <c r="A37" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:L3PredictiveDigitalTwin</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="11" t="str">
+      <c r="B37" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v>ditta:L2InformativeDigitalTwin</v>
+      </c>
+      <c r="G37" s="13" t="str">
         <f t="shared" si="7"/>
-        <v>ditta:L2InformativeDigitalTwin</v>
-      </c>
-      <c r="G33" s="11" t="str">
-        <f t="shared" si="6"/>
         <v>ditta:Simulation-PredictionDigitalTwin</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="11" t="str">
+    <row r="38">
+      <c r="A38" s="13" t="str">
         <f t="shared" si="1"/>
         <v>ditta:L4LivingDigitalTwin</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="11" t="str">
-        <f t="shared" si="7"/>
+      <c r="B38" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="13" t="str">
+        <f t="shared" si="8"/>
         <v>ditta:L3PredictiveDigitalTwin</v>
       </c>
-      <c r="G34" s="11" t="str">
-        <f>TEXTJOIN(",",1,A28,A29,A30,A40,A41)</f>
+      <c r="G38" s="13" t="str">
+        <f>TEXTJOIN(",",1,A32,A33,A34,A44,A45)</f>
         <v>ditta:Intelligent-LearningDigitalTwin,ditta:AutonomousDigitalTwin,ditta:CognitiveDigitalTwin,ditta:5-AutonomousDigitalTwin,ditta:IntelligentDigitalTwin</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" s="11" t="str">
-        <f>$A$24</f>
+    <row r="39">
+      <c r="A39" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="13" t="str">
+        <f>$A$28</f>
         <v>ditta:SystemFunctionality</v>
       </c>
-      <c r="G35" s="11" t="str">
-        <f>A51</f>
+      <c r="G39" s="13" t="str">
+        <f>A55</f>
         <v>ditta:DigitalTwinPrototype</v>
       </c>
-      <c r="I35" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="K35" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="11" t="str">
-        <f t="shared" ref="E36:E40" si="8">A35</f>
+      <c r="I39" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="K39" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="13" t="str">
+        <f t="shared" ref="E40:E44" si="9">A39</f>
         <v>ditta:0-StandaloneDigitalTwin</v>
       </c>
-      <c r="G36" s="11" t="str">
-        <f t="shared" ref="G36:G38" si="9">TEXTJOIN(",",1,A31,A25)</f>
+      <c r="G40" s="13" t="str">
+        <f t="shared" ref="G40:G42" si="10">TEXTJOIN(",",1,A35,A29)</f>
         <v>ditta:L1DescriptiveDigitalTwin,ditta:SupervisoryDigitalTwin</v>
       </c>
-      <c r="I36" s="17" t="str">
-        <f t="shared" ref="I36:I40" si="10">I35</f>
+      <c r="I40" s="19" t="str">
+        <f t="shared" ref="I40:I44" si="11">I39</f>
         <v>https://orcid.org/0009-0003-5155-0870</v>
       </c>
-      <c r="K36" s="17" t="str">
-        <f t="shared" ref="K36:K40" si="11">K35</f>
+      <c r="K40" s="19" t="str">
+        <f t="shared" ref="K40:K44" si="12">K39</f>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="11" t="str">
-        <f t="shared" si="8"/>
+    <row r="41">
+      <c r="A41" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="13" t="str">
+        <f t="shared" si="9"/>
         <v>ditta:1-DescriptiveDigitalTwin</v>
       </c>
-      <c r="G37" s="11" t="str">
+      <c r="G41" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>ditta:L2InformativeDigitalTwin,ditta:OperationalDigitalTwin</v>
+      </c>
+      <c r="I41" s="19" t="str">
+        <f t="shared" si="11"/>
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K41" s="19" t="str">
+        <f t="shared" si="12"/>
+        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" s="13" t="str">
         <f t="shared" si="9"/>
-        <v>ditta:L2InformativeDigitalTwin,ditta:OperationalDigitalTwin</v>
-      </c>
-      <c r="I37" s="17" t="str">
+        <v>ditta:2-DiagnosticDigitalTwin</v>
+      </c>
+      <c r="G42" s="13" t="str">
         <f t="shared" si="10"/>
+        <v>ditta:L3PredictiveDigitalTwin,ditta:Simulation-PredictionDigitalTwin</v>
+      </c>
+      <c r="I42" s="19" t="str">
+        <f t="shared" si="11"/>
         <v>https://orcid.org/0009-0003-5155-0870</v>
       </c>
-      <c r="K37" s="17" t="str">
+      <c r="K42" s="19" t="str">
+        <f t="shared" si="12"/>
+        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>ditta:3-PredictiveDigitalTwin</v>
+      </c>
+      <c r="G43" s="13" t="str">
+        <f>TEXTJOIN(",",1,A38,A32, A45)</f>
+        <v>ditta:L4LivingDigitalTwin,ditta:Intelligent-LearningDigitalTwin,ditta:IntelligentDigitalTwin</v>
+      </c>
+      <c r="I43" s="19" t="str">
         <f t="shared" si="11"/>
+        <v>https://orcid.org/0009-0003-5155-0870</v>
+      </c>
+      <c r="K43" s="19" t="str">
+        <f t="shared" si="12"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v>ditta:2-DiagnosticDigitalTwin</v>
-      </c>
-      <c r="G38" s="11" t="str">
+    <row r="44">
+      <c r="A44" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="13" t="str">
         <f t="shared" si="9"/>
-        <v>ditta:L3PredictiveDigitalTwin,ditta:Simulation-PredictionDigitalTwin</v>
-      </c>
-      <c r="I38" s="17" t="str">
-        <f t="shared" si="10"/>
+        <v>ditta:4-PrescriptiveDigitalTwin</v>
+      </c>
+      <c r="F44" s="13" t="str">
+        <f>TEXTJOIN(",",1,A33)</f>
+        <v>ditta:AutonomousDigitalTwin</v>
+      </c>
+      <c r="G44" s="13" t="str">
+        <f>TEXTJOIN(",",1,A34,A38,A45)</f>
+        <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:IntelligentDigitalTwin</v>
+      </c>
+      <c r="I44" s="19" t="str">
+        <f t="shared" si="11"/>
         <v>https://orcid.org/0009-0003-5155-0870</v>
       </c>
-      <c r="K38" s="17" t="str">
-        <f t="shared" si="11"/>
+      <c r="K44" s="19" t="str">
+        <f t="shared" si="12"/>
         <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v>ditta:3-PredictiveDigitalTwin</v>
-      </c>
-      <c r="G39" s="11" t="str">
-        <f>TEXTJOIN(",",1,A34,A28, A41)</f>
-        <v>ditta:L4LivingDigitalTwin,ditta:Intelligent-LearningDigitalTwin,ditta:IntelligentDigitalTwin</v>
-      </c>
-      <c r="I39" s="17" t="str">
-        <f t="shared" si="10"/>
-        <v>https://orcid.org/0009-0003-5155-0870</v>
-      </c>
-      <c r="K39" s="17" t="str">
-        <f t="shared" si="11"/>
-        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E40" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v>ditta:4-PrescriptiveDigitalTwin</v>
-      </c>
-      <c r="F40" s="11" t="str">
-        <f>TEXTJOIN(",",1,A29)</f>
-        <v>ditta:AutonomousDigitalTwin</v>
-      </c>
-      <c r="G40" s="11" t="str">
-        <f>TEXTJOIN(",",1,A30,A34,A41)</f>
-        <v>ditta:CognitiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:IntelligentDigitalTwin</v>
-      </c>
-      <c r="I40" s="17" t="str">
-        <f t="shared" si="10"/>
-        <v>https://orcid.org/0009-0003-5155-0870</v>
-      </c>
-      <c r="K40" s="17" t="str">
-        <f t="shared" si="11"/>
-        <v>https://doi.org/10.1109/ACCESS.2023.3321320</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="11" t="str">
-        <f t="shared" ref="A41:A53" si="12">IF(ISBLANK($B41),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B41," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+    <row r="45">
+      <c r="A45" s="13" t="str">
+        <f t="shared" ref="A45:A60" si="13">IF(ISBLANK($B45),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B45," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>ditta:IntelligentDigitalTwin</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="11" t="str">
-        <f>$A$24</f>
+      <c r="B45" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="14"/>
+      <c r="E45" s="13" t="str">
+        <f>$A$28</f>
         <v>ditta:SystemFunctionality</v>
       </c>
-      <c r="G41" s="11" t="str">
-        <f>TEXTJOIN(",",1,A28,A40,A39,A34,A29)</f>
+      <c r="G45" s="13" t="str">
+        <f>TEXTJOIN(",",1,A32,A44,A43,A38,A33)</f>
         <v>ditta:Intelligent-LearningDigitalTwin,ditta:5-AutonomousDigitalTwin,ditta:4-PrescriptiveDigitalTwin,ditta:L4LivingDigitalTwin,ditta:AutonomousDigitalTwin</v>
       </c>
-      <c r="I41" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K41" s="14" t="s">
+      <c r="I45" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="11" t="str">
-        <f t="shared" si="12"/>
+      <c r="K45" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="13" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:ConnectionSystemAutomation</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E42" s="11" t="str">
+      <c r="B46" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" s="13" t="str">
         <f>$A$17</f>
         <v>ditta:DigitalTwinType</v>
       </c>
-      <c r="H42" s="11" t="str">
+      <c r="H46" s="13" t="str">
         <f>A20</f>
         <v>ditta:ConnectionSystem</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="11" t="str">
-        <f t="shared" si="12"/>
-        <v>ditta:ManuallyCoupledDigitalTwin</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="E43" s="11" t="str">
-        <f t="shared" ref="E43:E45" si="13">A42</f>
-        <v>ditta:ConnectionSystemAutomation</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="J43" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K43" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="L43" s="12"/>
-      <c r="N43" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="11" t="str">
-        <f t="shared" si="12"/>
-        <v>ditta:DigitalShadow</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E44" s="11" t="str">
+    <row r="47">
+      <c r="A47" s="13" t="str">
         <f t="shared" si="13"/>
         <v>ditta:ManuallyCoupledDigitalTwin</v>
       </c>
-      <c r="I44" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="J44" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K44" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="L44" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="N44" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="11" t="str">
-        <f t="shared" si="12"/>
-        <v>ditta:FullyCoupledDigitalTwin</v>
-      </c>
-      <c r="B45" s="12" t="s">
+      <c r="B47" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C47" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D47" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="E45" s="11" t="str">
+      <c r="E47" s="13" t="str">
+        <f t="shared" ref="E47:E49" si="14">A46</f>
+        <v>ditta:ConnectionSystemAutomation</v>
+      </c>
+      <c r="I47" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="L47" s="14"/>
+      <c r="N47" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="13" t="str">
         <f t="shared" si="13"/>
         <v>ditta:DigitalShadow</v>
       </c>
-      <c r="I45" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="J45" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K45" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="L45" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="N45" s="12" t="s">
+      <c r="B48" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" s="13" t="str">
+        <f t="shared" si="14"/>
+        <v>ditta:ManuallyCoupledDigitalTwin</v>
+      </c>
+      <c r="I48" s="17" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="11" t="str">
-        <f t="shared" si="12"/>
+      <c r="J48" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K48" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="L48" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N48" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="13" t="str">
+        <f t="shared" si="13"/>
+        <v>ditta:FullyCoupledDigitalTwin</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E49" s="13" t="str">
+        <f t="shared" si="14"/>
+        <v>ditta:DigitalShadow</v>
+      </c>
+      <c r="I49" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K49" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N49" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="13" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:ModelFidelity</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="E46" s="11" t="str">
+      <c r="B50" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="13" t="str">
         <f>$A$17</f>
         <v>ditta:DigitalTwinType</v>
       </c>
-      <c r="H46" s="11" t="str">
+      <c r="H50" s="13" t="str">
         <f>$A$21</f>
         <v>ditta:ModelSystem</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="11" t="str">
-        <f t="shared" si="12"/>
+    <row r="51">
+      <c r="A51" s="13" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:LowFidelityDigitalTwin</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E47" s="11" t="str">
-        <f t="shared" ref="E47:E49" si="14">$A$46</f>
+      <c r="B51" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="13" t="str">
+        <f t="shared" ref="E51:E53" si="15">$A$50</f>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="11" t="str">
-        <f t="shared" si="12"/>
+    <row r="52">
+      <c r="A52" s="13" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:HighFidelityDigitalTwin</v>
       </c>
-      <c r="B48" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E48" s="11" t="str">
-        <f t="shared" si="14"/>
+      <c r="B52" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E52" s="13" t="str">
+        <f t="shared" si="15"/>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="11" t="str">
-        <f t="shared" si="12"/>
+    <row r="53">
+      <c r="A53" s="13" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:Multi-FidelityDigitalTwin</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E49" s="11" t="str">
-        <f t="shared" si="14"/>
+      <c r="B53" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E53" s="13" t="str">
+        <f t="shared" si="15"/>
         <v>ditta:ModelFidelity</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="11" t="str">
-        <f t="shared" si="12"/>
+    <row r="54">
+      <c r="A54" s="13" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
-      <c r="B50" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E50" s="11" t="str">
+      <c r="B54" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E54" s="13" t="str">
         <f>$A$17</f>
         <v>ditta:DigitalTwinType</v>
       </c>
-      <c r="H50" s="11" t="str">
+      <c r="H54" s="13" t="str">
         <f>$A$18</f>
         <v>ditta:PhysicalSystem</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="11" t="str">
-        <f t="shared" si="12"/>
+    <row r="55">
+      <c r="A55" s="13" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:DigitalTwinPrototype</v>
       </c>
-      <c r="B51" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="E51" s="11" t="str">
-        <f t="shared" ref="E51:E53" si="15">$A$50</f>
+      <c r="B55" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E55" s="13" t="str">
+        <f t="shared" ref="E55:E57" si="16">$A$54</f>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
-      <c r="I51" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K51" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="11" t="str">
-        <f t="shared" si="12"/>
+      <c r="I55" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K55" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="13" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:DigitalTwinInstance</v>
       </c>
-      <c r="B52" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="E52" s="11" t="str">
-        <f t="shared" si="15"/>
+      <c r="B56" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" s="13" t="str">
+        <f t="shared" si="16"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
-      <c r="I52" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K52" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="11" t="str">
-        <f t="shared" si="12"/>
+      <c r="I56" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K56" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="13" t="str">
+        <f t="shared" si="13"/>
         <v>ditta:DigitalTwinAggregate</v>
       </c>
-      <c r="B53" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E53" s="11" t="str">
-        <f t="shared" si="15"/>
+      <c r="B57" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" s="13" t="str">
+        <f t="shared" si="16"/>
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
-      <c r="I53" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K53" s="14" t="s">
+      <c r="I57" s="16" t="s">
         <v>38</v>
+      </c>
+      <c r="K57" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="13" t="str">
+        <f t="shared" si="13"/>
+        <v>ditta:ConceptualModelDimensionality</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E58" s="13" t="str">
+        <f>A17</f>
+        <v>ditta:DigitalTwinType</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="13" t="str">
+        <f t="shared" si="13"/>
+        <v>ditta:Three-dimensionalDigitalTwin</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E59" s="13" t="str">
+        <f>A58</f>
+        <v>ditta:ConceptualModelDimensionality</v>
+      </c>
+      <c r="F59" s="13" t="str">
+        <f>A16</f>
+        <v>ditta:DigitalTwinConceptualModel</v>
+      </c>
+      <c r="I59" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="13" t="str">
+        <f t="shared" si="13"/>
+        <v>ditta:Five-dimensionalDigitalTwin</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E60" s="13" t="str">
+        <f>A58</f>
+        <v>ditta:ConceptualModelDimensionality</v>
+      </c>
+      <c r="I60" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1885,48 +2101,64 @@
     <hyperlink r:id="rId1" ref="B1"/>
     <hyperlink r:id="rId2" ref="C2"/>
     <hyperlink r:id="rId3" ref="C3"/>
-    <hyperlink r:id="rId4" ref="C4"/>
-    <hyperlink r:id="rId5" ref="B8"/>
-    <hyperlink r:id="rId6" ref="B9"/>
+    <hyperlink r:id="rId4" ref="B8"/>
+    <hyperlink r:id="rId5" ref="B10"/>
+    <hyperlink r:id="rId6" ref="B11"/>
     <hyperlink r:id="rId7" ref="I16"/>
     <hyperlink r:id="rId8" ref="K16"/>
     <hyperlink r:id="rId9" ref="I17"/>
     <hyperlink r:id="rId10" ref="I18"/>
     <hyperlink r:id="rId11" ref="I19"/>
     <hyperlink r:id="rId12" ref="I20"/>
-    <hyperlink r:id="rId13" ref="I26"/>
-    <hyperlink r:id="rId14" ref="K26"/>
-    <hyperlink r:id="rId15" ref="I27"/>
-    <hyperlink r:id="rId16" ref="K27"/>
-    <hyperlink r:id="rId17" ref="I28"/>
-    <hyperlink r:id="rId18" ref="K28"/>
-    <hyperlink r:id="rId19" ref="I29"/>
-    <hyperlink r:id="rId20" ref="K29"/>
-    <hyperlink r:id="rId21" ref="I30"/>
-    <hyperlink r:id="rId22" ref="K30"/>
-    <hyperlink r:id="rId23" ref="L30"/>
-    <hyperlink r:id="rId24" ref="I35"/>
-    <hyperlink r:id="rId25" ref="K35"/>
-    <hyperlink r:id="rId26" ref="I41"/>
-    <hyperlink r:id="rId27" ref="K41"/>
-    <hyperlink r:id="rId28" ref="I43"/>
-    <hyperlink r:id="rId29" ref="J43"/>
-    <hyperlink r:id="rId30" ref="K43"/>
-    <hyperlink r:id="rId31" ref="I44"/>
-    <hyperlink r:id="rId32" ref="J44"/>
-    <hyperlink r:id="rId33" ref="K44"/>
-    <hyperlink r:id="rId34" ref="L44"/>
-    <hyperlink r:id="rId35" ref="I45"/>
-    <hyperlink r:id="rId36" ref="J45"/>
-    <hyperlink r:id="rId37" ref="K45"/>
-    <hyperlink r:id="rId38" ref="L45"/>
-    <hyperlink r:id="rId39" ref="I51"/>
-    <hyperlink r:id="rId40" ref="K51"/>
-    <hyperlink r:id="rId41" ref="I52"/>
-    <hyperlink r:id="rId42" ref="K52"/>
-    <hyperlink r:id="rId43" ref="I53"/>
-    <hyperlink r:id="rId44" ref="K53"/>
+    <hyperlink r:id="rId13" ref="I21"/>
+    <hyperlink r:id="rId14" ref="K21"/>
+    <hyperlink r:id="rId15" ref="I22"/>
+    <hyperlink r:id="rId16" ref="K22"/>
+    <hyperlink r:id="rId17" ref="I23"/>
+    <hyperlink r:id="rId18" ref="K23"/>
+    <hyperlink r:id="rId19" ref="I24"/>
+    <hyperlink r:id="rId20" ref="K24"/>
+    <hyperlink r:id="rId21" ref="I25"/>
+    <hyperlink r:id="rId22" ref="K25"/>
+    <hyperlink r:id="rId23" ref="I26"/>
+    <hyperlink r:id="rId24" ref="K26"/>
+    <hyperlink r:id="rId25" ref="I27"/>
+    <hyperlink r:id="rId26" ref="K27"/>
+    <hyperlink r:id="rId27" ref="I30"/>
+    <hyperlink r:id="rId28" ref="K30"/>
+    <hyperlink r:id="rId29" ref="I31"/>
+    <hyperlink r:id="rId30" ref="K31"/>
+    <hyperlink r:id="rId31" ref="I32"/>
+    <hyperlink r:id="rId32" ref="K32"/>
+    <hyperlink r:id="rId33" ref="I33"/>
+    <hyperlink r:id="rId34" ref="K33"/>
+    <hyperlink r:id="rId35" ref="I34"/>
+    <hyperlink r:id="rId36" ref="K34"/>
+    <hyperlink r:id="rId37" ref="L34"/>
+    <hyperlink r:id="rId38" ref="I39"/>
+    <hyperlink r:id="rId39" ref="K39"/>
+    <hyperlink r:id="rId40" ref="I45"/>
+    <hyperlink r:id="rId41" ref="K45"/>
+    <hyperlink r:id="rId42" ref="I47"/>
+    <hyperlink r:id="rId43" ref="J47"/>
+    <hyperlink r:id="rId44" ref="K47"/>
+    <hyperlink r:id="rId45" ref="I48"/>
+    <hyperlink r:id="rId46" ref="J48"/>
+    <hyperlink r:id="rId47" ref="K48"/>
+    <hyperlink r:id="rId48" ref="L48"/>
+    <hyperlink r:id="rId49" ref="I49"/>
+    <hyperlink r:id="rId50" ref="J49"/>
+    <hyperlink r:id="rId51" ref="K49"/>
+    <hyperlink r:id="rId52" ref="L49"/>
+    <hyperlink r:id="rId53" ref="I55"/>
+    <hyperlink r:id="rId54" ref="K55"/>
+    <hyperlink r:id="rId55" ref="I56"/>
+    <hyperlink r:id="rId56" ref="K56"/>
+    <hyperlink r:id="rId57" ref="I57"/>
+    <hyperlink r:id="rId58" ref="K57"/>
+    <hyperlink r:id="rId59" ref="I59"/>
+    <hyperlink r:id="rId60" ref="I60"/>
   </hyperlinks>
-  <drawing r:id="rId45"/>
+  <drawing r:id="rId61"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ENH:Add digital shadow synonym
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -11,20 +11,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="136">
   <si>
     <t>ConceptScheme URI</t>
   </si>
   <si>
-    <t>https://www.rtdt.ai/ontologies/digital-twin-taxonomy/</t>
-  </si>
-  <si>
     <t>PREFIX</t>
   </si>
   <si>
     <t>ditta</t>
   </si>
   <si>
+    <t>https://www.w3id.org/ontoforge/digital-twin-taxonomy/</t>
+  </si>
+  <si>
     <t>dct</t>
   </si>
   <si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t xml:space="preserve">A Digital Shadow is a digital representation of an existing or planned physical object with an automated one-way data flow between a physical object and a digital object. </t>
+  </si>
+  <si>
+    <t>One-way Coupled Digital Twin</t>
   </si>
   <si>
     <t>As opposed to Kritzinger et al.(2018), this definition does not state that the physical object should exist. See: Grieves, M.: Intelligent digital twins and the development and management of complex systems, 2022.</t>
@@ -776,8 +779,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="29.88"/>
-    <col customWidth="1" min="2" max="2" width="40.0"/>
+    <col customWidth="1" min="2" max="2" width="41.38"/>
     <col customWidth="1" min="3" max="3" width="54.88"/>
+    <col customWidth="1" min="4" max="4" width="16.63"/>
     <col customWidth="1" min="5" max="5" width="29.5"/>
     <col customWidth="1" min="7" max="7" width="67.75"/>
     <col customWidth="1" min="9" max="9" width="30.5"/>
@@ -789,8 +793,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="str">
+        <f>C2</f>
+        <v>https://www.w3id.org/ontoforge/digital-twin-taxonomy/</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -807,13 +812,13 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -829,7 +834,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -851,7 +856,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
@@ -1849,7 +1854,7 @@
         <v>113</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E48" s="13" t="str">
         <f t="shared" si="14"/>
@@ -1868,7 +1873,7 @@
         <v>39</v>
       </c>
       <c r="N48" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49">
@@ -1877,13 +1882,13 @@
         <v>ditta:FullyCoupledDigitalTwin</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E49" s="13" t="str">
         <f t="shared" si="14"/>
@@ -1902,7 +1907,7 @@
         <v>39</v>
       </c>
       <c r="N49" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50">
@@ -1911,7 +1916,7 @@
         <v>ditta:ModelFidelity</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E50" s="13" t="str">
         <f>$A$17</f>
@@ -1928,7 +1933,7 @@
         <v>ditta:LowFidelityDigitalTwin</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E51" s="13" t="str">
         <f t="shared" ref="E51:E53" si="15">$A$50</f>
@@ -1941,7 +1946,7 @@
         <v>ditta:HighFidelityDigitalTwin</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E52" s="13" t="str">
         <f t="shared" si="15"/>
@@ -1954,7 +1959,7 @@
         <v>ditta:Multi-FidelityDigitalTwin</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E53" s="13" t="str">
         <f t="shared" si="15"/>
@@ -1967,7 +1972,7 @@
         <v>ditta:PhysicalSystemLifetimeStage</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E54" s="13" t="str">
         <f>$A$17</f>
@@ -1984,10 +1989,10 @@
         <v>ditta:DigitalTwinPrototype</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E55" s="13" t="str">
         <f t="shared" ref="E55:E57" si="16">$A$54</f>
@@ -1997,7 +2002,7 @@
         <v>38</v>
       </c>
       <c r="K55" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56">
@@ -2006,10 +2011,10 @@
         <v>ditta:DigitalTwinInstance</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E56" s="13" t="str">
         <f t="shared" si="16"/>
@@ -2019,7 +2024,7 @@
         <v>38</v>
       </c>
       <c r="K56" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57">
@@ -2028,10 +2033,10 @@
         <v>ditta:DigitalTwinAggregate</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E57" s="13" t="str">
         <f t="shared" si="16"/>
@@ -2050,7 +2055,7 @@
         <v>ditta:ConceptualModelDimensionality</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E58" s="13" t="str">
         <f>A17</f>
@@ -2063,7 +2068,7 @@
         <v>ditta:Three-dimensionalDigitalTwin</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E59" s="13" t="str">
         <f>A58</f>
@@ -2083,10 +2088,10 @@
         <v>ditta:Five-dimensionalDigitalTwin</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E60" s="13" t="str">
         <f>A58</f>
@@ -2098,67 +2103,66 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B1"/>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="C3"/>
-    <hyperlink r:id="rId4" ref="B8"/>
-    <hyperlink r:id="rId5" ref="B10"/>
-    <hyperlink r:id="rId6" ref="B11"/>
-    <hyperlink r:id="rId7" ref="I16"/>
-    <hyperlink r:id="rId8" ref="K16"/>
-    <hyperlink r:id="rId9" ref="I17"/>
-    <hyperlink r:id="rId10" ref="I18"/>
-    <hyperlink r:id="rId11" ref="I19"/>
-    <hyperlink r:id="rId12" ref="I20"/>
-    <hyperlink r:id="rId13" ref="I21"/>
-    <hyperlink r:id="rId14" ref="K21"/>
-    <hyperlink r:id="rId15" ref="I22"/>
-    <hyperlink r:id="rId16" ref="K22"/>
-    <hyperlink r:id="rId17" ref="I23"/>
-    <hyperlink r:id="rId18" ref="K23"/>
-    <hyperlink r:id="rId19" ref="I24"/>
-    <hyperlink r:id="rId20" ref="K24"/>
-    <hyperlink r:id="rId21" ref="I25"/>
-    <hyperlink r:id="rId22" ref="K25"/>
-    <hyperlink r:id="rId23" ref="I26"/>
-    <hyperlink r:id="rId24" ref="K26"/>
-    <hyperlink r:id="rId25" ref="I27"/>
-    <hyperlink r:id="rId26" ref="K27"/>
-    <hyperlink r:id="rId27" ref="I30"/>
-    <hyperlink r:id="rId28" ref="K30"/>
-    <hyperlink r:id="rId29" ref="I31"/>
-    <hyperlink r:id="rId30" ref="K31"/>
-    <hyperlink r:id="rId31" ref="I32"/>
-    <hyperlink r:id="rId32" ref="K32"/>
-    <hyperlink r:id="rId33" ref="I33"/>
-    <hyperlink r:id="rId34" ref="K33"/>
-    <hyperlink r:id="rId35" ref="I34"/>
-    <hyperlink r:id="rId36" ref="K34"/>
-    <hyperlink r:id="rId37" ref="L34"/>
-    <hyperlink r:id="rId38" ref="I39"/>
-    <hyperlink r:id="rId39" ref="K39"/>
-    <hyperlink r:id="rId40" ref="I45"/>
-    <hyperlink r:id="rId41" ref="K45"/>
-    <hyperlink r:id="rId42" ref="I47"/>
-    <hyperlink r:id="rId43" ref="J47"/>
-    <hyperlink r:id="rId44" ref="K47"/>
-    <hyperlink r:id="rId45" ref="I48"/>
-    <hyperlink r:id="rId46" ref="J48"/>
-    <hyperlink r:id="rId47" ref="K48"/>
-    <hyperlink r:id="rId48" ref="L48"/>
-    <hyperlink r:id="rId49" ref="I49"/>
-    <hyperlink r:id="rId50" ref="J49"/>
-    <hyperlink r:id="rId51" ref="K49"/>
-    <hyperlink r:id="rId52" ref="L49"/>
-    <hyperlink r:id="rId53" ref="I55"/>
-    <hyperlink r:id="rId54" ref="K55"/>
-    <hyperlink r:id="rId55" ref="I56"/>
-    <hyperlink r:id="rId56" ref="K56"/>
-    <hyperlink r:id="rId57" ref="I57"/>
-    <hyperlink r:id="rId58" ref="K57"/>
-    <hyperlink r:id="rId59" ref="I59"/>
-    <hyperlink r:id="rId60" ref="I60"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="B8"/>
+    <hyperlink r:id="rId4" ref="B10"/>
+    <hyperlink r:id="rId5" ref="B11"/>
+    <hyperlink r:id="rId6" ref="I16"/>
+    <hyperlink r:id="rId7" ref="K16"/>
+    <hyperlink r:id="rId8" ref="I17"/>
+    <hyperlink r:id="rId9" ref="I18"/>
+    <hyperlink r:id="rId10" ref="I19"/>
+    <hyperlink r:id="rId11" ref="I20"/>
+    <hyperlink r:id="rId12" ref="I21"/>
+    <hyperlink r:id="rId13" ref="K21"/>
+    <hyperlink r:id="rId14" ref="I22"/>
+    <hyperlink r:id="rId15" ref="K22"/>
+    <hyperlink r:id="rId16" ref="I23"/>
+    <hyperlink r:id="rId17" ref="K23"/>
+    <hyperlink r:id="rId18" ref="I24"/>
+    <hyperlink r:id="rId19" ref="K24"/>
+    <hyperlink r:id="rId20" ref="I25"/>
+    <hyperlink r:id="rId21" ref="K25"/>
+    <hyperlink r:id="rId22" ref="I26"/>
+    <hyperlink r:id="rId23" ref="K26"/>
+    <hyperlink r:id="rId24" ref="I27"/>
+    <hyperlink r:id="rId25" ref="K27"/>
+    <hyperlink r:id="rId26" ref="I30"/>
+    <hyperlink r:id="rId27" ref="K30"/>
+    <hyperlink r:id="rId28" ref="I31"/>
+    <hyperlink r:id="rId29" ref="K31"/>
+    <hyperlink r:id="rId30" ref="I32"/>
+    <hyperlink r:id="rId31" ref="K32"/>
+    <hyperlink r:id="rId32" ref="I33"/>
+    <hyperlink r:id="rId33" ref="K33"/>
+    <hyperlink r:id="rId34" ref="I34"/>
+    <hyperlink r:id="rId35" ref="K34"/>
+    <hyperlink r:id="rId36" ref="L34"/>
+    <hyperlink r:id="rId37" ref="I39"/>
+    <hyperlink r:id="rId38" ref="K39"/>
+    <hyperlink r:id="rId39" ref="I45"/>
+    <hyperlink r:id="rId40" ref="K45"/>
+    <hyperlink r:id="rId41" ref="I47"/>
+    <hyperlink r:id="rId42" ref="J47"/>
+    <hyperlink r:id="rId43" ref="K47"/>
+    <hyperlink r:id="rId44" ref="I48"/>
+    <hyperlink r:id="rId45" ref="J48"/>
+    <hyperlink r:id="rId46" ref="K48"/>
+    <hyperlink r:id="rId47" ref="L48"/>
+    <hyperlink r:id="rId48" ref="I49"/>
+    <hyperlink r:id="rId49" ref="J49"/>
+    <hyperlink r:id="rId50" ref="K49"/>
+    <hyperlink r:id="rId51" ref="L49"/>
+    <hyperlink r:id="rId52" ref="I55"/>
+    <hyperlink r:id="rId53" ref="K55"/>
+    <hyperlink r:id="rId54" ref="I56"/>
+    <hyperlink r:id="rId55" ref="K56"/>
+    <hyperlink r:id="rId56" ref="I57"/>
+    <hyperlink r:id="rId57" ref="K57"/>
+    <hyperlink r:id="rId58" ref="I59"/>
+    <hyperlink r:id="rId59" ref="I60"/>
   </hyperlinks>
-  <drawing r:id="rId61"/>
+  <drawing r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>